<commit_message>
Excel challenge 259 solution has been added.
</commit_message>
<xml_diff>
--- a/Excel Files/PQ Challenges/PQ  Challenge103 Problem.xlsx
+++ b/Excel Files/PQ Challenges/PQ  Challenge103 Problem.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Repositories\Excel-BI-Python\Excel Files\PQ Challenges\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93185B48-1653-4B25-856C-1591B6666B1D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65FF227D-C38F-4EF8-A6B2-65323B339F49}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="34620" windowHeight="14020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -958,6 +958,9 @@
   <we:bindings/>
   <we:snapshot xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships"/>
   <we:extLst>
+    <a:ext xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" uri="{D87F86FE-615C-45B5-9D79-34F1136793EB}">
+      <we:containsCustomFunctions/>
+    </a:ext>
     <a:ext xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" uri="{7C84B067-C214-45C3-A712-C9D94CD141B2}">
       <we:customFunctionIdList>
         <we:customFunctionIds>_xldudf_LABS_GENERATIVEAI</we:customFunctionIds>
@@ -973,7 +976,7 @@
   <dimension ref="A1:S16"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q1" sqref="Q1"/>
+      <selection activeCell="R5" sqref="R5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>